<commit_message>
fixed export and now connection to database only throught dbsettinggs parametres
</commit_message>
<xml_diff>
--- a/one_unique_organisations.xlsx
+++ b/one_unique_organisations.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:C31"/>
+  <dimension ref="A1:C70"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -451,7 +451,7 @@
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>533</t>
+          <t>4750</t>
         </is>
       </c>
       <c r="C2" t="inlineStr">
@@ -466,7 +466,7 @@
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>898</t>
+          <t>500</t>
         </is>
       </c>
       <c r="C3" t="inlineStr">
@@ -481,7 +481,7 @@
       </c>
       <c r="B4" t="inlineStr">
         <is>
-          <t>870</t>
+          <t>509</t>
         </is>
       </c>
       <c r="C4" t="inlineStr">
@@ -496,12 +496,12 @@
       </c>
       <c r="B5" t="inlineStr">
         <is>
-          <t>848</t>
+          <t>522</t>
         </is>
       </c>
       <c r="C5" t="inlineStr">
         <is>
-          <t>ООО «Газпромнефть НТЦ»</t>
+          <t>АО “Российские космические системы”</t>
         </is>
       </c>
     </row>
@@ -511,12 +511,12 @@
       </c>
       <c r="B6" t="inlineStr">
         <is>
-          <t>80</t>
+          <t>533</t>
         </is>
       </c>
       <c r="C6" t="inlineStr">
         <is>
-          <t>Institute of Earthquake Prediction Theory and Mathematical Geophysics|Russian Academy of Sciences</t>
+          <t>ООО «Газпромнефть НТЦ»</t>
         </is>
       </c>
     </row>
@@ -526,12 +526,12 @@
       </c>
       <c r="B7" t="inlineStr">
         <is>
-          <t>7655</t>
+          <t>549</t>
         </is>
       </c>
       <c r="C7" t="inlineStr">
         <is>
-          <t>ПАО «Татнефть»</t>
+          <t>Филиал ООО "ЛУКОЙЛ-Инжиниринг" "КогалымНИПИнефть" в г. Тюмени</t>
         </is>
       </c>
     </row>
@@ -541,12 +541,12 @@
       </c>
       <c r="B8" t="inlineStr">
         <is>
-          <t>734</t>
+          <t>570</t>
         </is>
       </c>
       <c r="C8" t="inlineStr">
         <is>
-          <t>Российский химико-технологический университет им. Д.И. Менделеева</t>
+          <t>ИПНГ РАН</t>
         </is>
       </c>
     </row>
@@ -556,12 +556,12 @@
       </c>
       <c r="B9" t="inlineStr">
         <is>
-          <t>7109</t>
+          <t>5932</t>
         </is>
       </c>
       <c r="C9" t="inlineStr">
         <is>
-          <t>ООО "Газпром ВНИИГАЗ"</t>
+          <t>I.M. Sechenov First Moscow State Medical University, the Ministry of Health of the Russian Federation (Sechenov University)</t>
         </is>
       </c>
     </row>
@@ -571,12 +571,12 @@
       </c>
       <c r="B10" t="inlineStr">
         <is>
-          <t>6939</t>
+          <t>6019</t>
         </is>
       </c>
       <c r="C10" t="inlineStr">
         <is>
-          <t>Institute of Marine Geology and Geophysics|Far East Branch|Russian Academy of Sciences</t>
+          <t>Институт теории прогноза землетрясений и математической геофизики РАН</t>
         </is>
       </c>
     </row>
@@ -586,12 +586,12 @@
       </c>
       <c r="B11" t="inlineStr">
         <is>
-          <t>570</t>
+          <t>6228</t>
         </is>
       </c>
       <c r="C11" t="inlineStr">
         <is>
-          <t>ИПНГ РАН</t>
+          <t>Almaty Institute of Power Engineering and Telecommunications</t>
         </is>
       </c>
     </row>
@@ -601,12 +601,12 @@
       </c>
       <c r="B12" t="inlineStr">
         <is>
-          <t>549</t>
+          <t>6317</t>
         </is>
       </c>
       <c r="C12" t="inlineStr">
         <is>
-          <t>Ухтинский государственный технический университет</t>
+          <t>НТС ПАО "Газпром"</t>
         </is>
       </c>
     </row>
@@ -616,12 +616,12 @@
       </c>
       <c r="B13" t="inlineStr">
         <is>
-          <t>500</t>
+          <t>6939</t>
         </is>
       </c>
       <c r="C13" t="inlineStr">
         <is>
-          <t>ФГАОУ ВО «Российский университет дружбы народов»</t>
+          <t>ПАО «Татнефть»</t>
         </is>
       </c>
     </row>
@@ -631,12 +631,12 @@
       </c>
       <c r="B14" t="inlineStr">
         <is>
-          <t>11374</t>
+          <t>7109</t>
         </is>
       </c>
       <c r="C14" t="inlineStr">
         <is>
-          <t>САФУ</t>
+          <t>ПАО «НК «Роснефть»</t>
         </is>
       </c>
     </row>
@@ -646,12 +646,12 @@
       </c>
       <c r="B15" t="inlineStr">
         <is>
-          <t>4750</t>
+          <t>734</t>
         </is>
       </c>
       <c r="C15" t="inlineStr">
         <is>
-          <t>ФГАОУ ВО «Тюменский государственный университет»</t>
+          <t>Ammosov North Eastern Federal University</t>
         </is>
       </c>
     </row>
@@ -661,12 +661,12 @@
       </c>
       <c r="B16" t="inlineStr">
         <is>
-          <t>4493</t>
+          <t>7655</t>
         </is>
       </c>
       <c r="C16" t="inlineStr">
         <is>
-          <t>Oil and Gas Research Institute|Russian Academy of Sciences (OGRI RAS)</t>
+          <t>Московский государственный университет им. М.В. Ломоносова</t>
         </is>
       </c>
     </row>
@@ -676,12 +676,12 @@
       </c>
       <c r="B17" t="inlineStr">
         <is>
-          <t>440</t>
+          <t>80</t>
         </is>
       </c>
       <c r="C17" t="inlineStr">
         <is>
-          <t>ВНИИОкеангеология</t>
+          <t>V.A. Trapeznikov Institute of Control Sciences|Russian Academy of Sciences</t>
         </is>
       </c>
     </row>
@@ -691,12 +691,12 @@
       </c>
       <c r="B18" t="inlineStr">
         <is>
-          <t>3966</t>
+          <t>848</t>
         </is>
       </c>
       <c r="C18" t="inlineStr">
         <is>
-          <t>ФГБУ «Всероссийский научно-исследовательский геологический нефтяной институт»</t>
+          <t>Institute of Geography RAS</t>
         </is>
       </c>
     </row>
@@ -706,12 +706,12 @@
       </c>
       <c r="B19" t="inlineStr">
         <is>
-          <t>364</t>
+          <t>870</t>
         </is>
       </c>
       <c r="C19" t="inlineStr">
         <is>
-          <t>V.B. Sochava Institute of Geography|Siberian Branch of Russian Academy of Sciences</t>
+          <t>The Moscow Mining University, NUSTMIS&amp;S</t>
         </is>
       </c>
     </row>
@@ -721,12 +721,12 @@
       </c>
       <c r="B20" t="inlineStr">
         <is>
-          <t>2268</t>
+          <t>898</t>
         </is>
       </c>
       <c r="C20" t="inlineStr">
         <is>
-          <t>Альметьевский государственный нефтяной институт</t>
+          <t>Российский химико-технологический университет им. Д.И. Менделеева</t>
         </is>
       </c>
     </row>
@@ -736,12 +736,12 @@
       </c>
       <c r="B21" t="inlineStr">
         <is>
-          <t>176</t>
+          <t>982</t>
         </is>
       </c>
       <c r="C21" t="inlineStr">
         <is>
-          <t>Frumkin Institute of Physical Chemistry and Electrochemistry|Russian Academy of Sciences</t>
+          <t>Институт микробиологии им. С.Н. Виноградского, ФИЦ Биотехнологии РАН</t>
         </is>
       </c>
     </row>
@@ -751,12 +751,12 @@
       </c>
       <c r="B22" t="inlineStr">
         <is>
-          <t>14552</t>
+          <t>4765</t>
         </is>
       </c>
       <c r="C22" t="inlineStr">
         <is>
-          <t>Пермский национальный исследовательский политехнический университет</t>
+          <t>Институт морской геологии и геофизики ДВО РАН</t>
         </is>
       </c>
     </row>
@@ -766,12 +766,12 @@
       </c>
       <c r="B23" t="inlineStr">
         <is>
-          <t>13814</t>
+          <t>452</t>
         </is>
       </c>
       <c r="C23" t="inlineStr">
         <is>
-          <t>Landau Institute for Theoretical Physics|RAS</t>
+          <t>Институт нефтехимического синтеза им. А.В. Топчиева РАН</t>
         </is>
       </c>
     </row>
@@ -781,12 +781,12 @@
       </c>
       <c r="B24" t="inlineStr">
         <is>
-          <t>132</t>
+          <t>11374</t>
         </is>
       </c>
       <c r="C24" t="inlineStr">
         <is>
-          <t>РГУ нефти и газа (НИУ) имени И.М. Губкина</t>
+          <t>Ухтинский государственный технический университет</t>
         </is>
       </c>
     </row>
@@ -796,12 +796,12 @@
       </c>
       <c r="B25" t="inlineStr">
         <is>
-          <t>982</t>
+          <t>440</t>
         </is>
       </c>
       <c r="C25" t="inlineStr">
         <is>
-          <t>Российский государственный геологоразведочный университет им. Серго Орджоникидзе</t>
+          <t>Norilsk State Industrial Institute</t>
         </is>
       </c>
     </row>
@@ -811,12 +811,12 @@
       </c>
       <c r="B26" t="inlineStr">
         <is>
-          <t xml:space="preserve"> </t>
+          <t>132</t>
         </is>
       </c>
       <c r="C26" t="inlineStr">
         <is>
-          <t>Department of Geography|The George Washington University</t>
+          <t>ФГАОУ ВО «Российский университет дружбы народов»</t>
         </is>
       </c>
     </row>
@@ -826,12 +826,12 @@
       </c>
       <c r="B27" t="inlineStr">
         <is>
-          <t xml:space="preserve"> </t>
+          <t>13814</t>
         </is>
       </c>
       <c r="C27" t="inlineStr">
         <is>
-          <t>ООО НТФ "Атомбиотех"</t>
+          <t>A.N. Nesmeyanov Institute of Organoelement Compounds of Russian Academy of Sciences</t>
         </is>
       </c>
     </row>
@@ -841,12 +841,12 @@
       </c>
       <c r="B28" t="inlineStr">
         <is>
-          <t xml:space="preserve"> </t>
+          <t>14430</t>
         </is>
       </c>
       <c r="C28" t="inlineStr">
         <is>
-          <t>Межотраслевой экспертно - аналитический центр Союза Нефтегазопромышленников России</t>
+          <t>Prokhorov General Physics Institute of the Russian Academy of Sciences</t>
         </is>
       </c>
     </row>
@@ -856,12 +856,12 @@
       </c>
       <c r="B29" t="inlineStr">
         <is>
-          <t xml:space="preserve"> </t>
+          <t>14552</t>
         </is>
       </c>
       <c r="C29" t="inlineStr">
         <is>
-          <t>ООО «Красноярскгазпром нефтегазпроект»</t>
+          <t>Northern (Arctic) Federal University named after M.V. Lomonosov</t>
         </is>
       </c>
     </row>
@@ -871,12 +871,12 @@
       </c>
       <c r="B30" t="inlineStr">
         <is>
-          <t xml:space="preserve"> </t>
+          <t>14819</t>
         </is>
       </c>
       <c r="C30" t="inlineStr">
         <is>
-          <t>ООО «КБ Стрелка»</t>
+          <t>Тюменский государственный университет</t>
         </is>
       </c>
     </row>
@@ -886,10 +886,595 @@
       </c>
       <c r="B31" t="inlineStr">
         <is>
-          <t xml:space="preserve"> </t>
+          <t>15203</t>
         </is>
       </c>
       <c r="C31" t="inlineStr">
+        <is>
+          <t>Институт проблем нефти и газа РАН</t>
+        </is>
+      </c>
+    </row>
+    <row r="32">
+      <c r="A32" s="1" t="n">
+        <v>30</v>
+      </c>
+      <c r="B32" t="inlineStr">
+        <is>
+          <t>162</t>
+        </is>
+      </c>
+      <c r="C32" t="inlineStr">
+        <is>
+          <t>Всероссийский научно-исследовательский геологический институт им. А.П. Карпинского</t>
+        </is>
+      </c>
+    </row>
+    <row r="33">
+      <c r="A33" s="1" t="n">
+        <v>31</v>
+      </c>
+      <c r="B33" t="inlineStr">
+        <is>
+          <t>176</t>
+        </is>
+      </c>
+      <c r="C33" t="inlineStr">
+        <is>
+          <t>ООО «Газпром добыча Надым»</t>
+        </is>
+      </c>
+    </row>
+    <row r="34">
+      <c r="A34" s="1" t="n">
+        <v>32</v>
+      </c>
+      <c r="B34" t="inlineStr">
+        <is>
+          <t>19244</t>
+        </is>
+      </c>
+      <c r="C34" t="inlineStr">
+        <is>
+          <t>ООО «РН-СахалинНИПИморнефть»</t>
+        </is>
+      </c>
+    </row>
+    <row r="35">
+      <c r="A35" s="1" t="n">
+        <v>33</v>
+      </c>
+      <c r="B35" t="inlineStr">
+        <is>
+          <t>2258</t>
+        </is>
+      </c>
+      <c r="C35" t="inlineStr">
+        <is>
+          <t>Институт криосферы Земли ТюмНЦ СО РАН</t>
+        </is>
+      </c>
+    </row>
+    <row r="36">
+      <c r="A36" s="1" t="n">
+        <v>34</v>
+      </c>
+      <c r="B36" t="inlineStr">
+        <is>
+          <t>2268</t>
+        </is>
+      </c>
+      <c r="C36" t="inlineStr">
+        <is>
+          <t>ВНИИОкеангеология</t>
+        </is>
+      </c>
+    </row>
+    <row r="37">
+      <c r="A37" s="1" t="n">
+        <v>35</v>
+      </c>
+      <c r="B37" t="inlineStr">
+        <is>
+          <t>2280</t>
+        </is>
+      </c>
+      <c r="C37" t="inlineStr">
+        <is>
+          <t>All-Russian Research Geological Oil Institute</t>
+        </is>
+      </c>
+    </row>
+    <row r="38">
+      <c r="A38" s="1" t="n">
+        <v>36</v>
+      </c>
+      <c r="B38" t="inlineStr">
+        <is>
+          <t>252</t>
+        </is>
+      </c>
+      <c r="C38" t="inlineStr">
+        <is>
+          <t>V.B. Sochava Institute of Geography|Siberian Branch of Russian Academy of Sciences</t>
+        </is>
+      </c>
+    </row>
+    <row r="39">
+      <c r="A39" s="1" t="n">
+        <v>37</v>
+      </c>
+      <c r="B39" t="inlineStr">
+        <is>
+          <t>2541</t>
+        </is>
+      </c>
+      <c r="C39" t="inlineStr">
+        <is>
+          <t>Альметьевский гос. нефтяной институт</t>
+        </is>
+      </c>
+    </row>
+    <row r="40">
+      <c r="A40" s="1" t="n">
+        <v>38</v>
+      </c>
+      <c r="B40" t="inlineStr">
+        <is>
+          <t>257</t>
+        </is>
+      </c>
+      <c r="C40" t="inlineStr">
+        <is>
+          <t>Frumkin Institute of Physical Chemistry and Electrochemistry|Russian Academy of Sciences</t>
+        </is>
+      </c>
+    </row>
+    <row r="41">
+      <c r="A41" s="1" t="n">
+        <v>39</v>
+      </c>
+      <c r="B41" t="inlineStr">
+        <is>
+          <t>327</t>
+        </is>
+      </c>
+      <c r="C41" t="inlineStr">
+        <is>
+          <t>Пермский национальный исследовательский политехнический университет</t>
+        </is>
+      </c>
+    </row>
+    <row r="42">
+      <c r="A42" s="1" t="n">
+        <v>40</v>
+      </c>
+      <c r="B42" t="inlineStr">
+        <is>
+          <t>361</t>
+        </is>
+      </c>
+      <c r="C42" t="inlineStr">
+        <is>
+          <t>Landau Institute for Theoretical Physics|Russian Academy of Sciences</t>
+        </is>
+      </c>
+    </row>
+    <row r="43">
+      <c r="A43" s="1" t="n">
+        <v>41</v>
+      </c>
+      <c r="B43" t="inlineStr">
+        <is>
+          <t>364</t>
+        </is>
+      </c>
+      <c r="C43" t="inlineStr">
+        <is>
+          <t>Gubkin University</t>
+        </is>
+      </c>
+    </row>
+    <row r="44">
+      <c r="A44" s="1" t="n">
+        <v>42</v>
+      </c>
+      <c r="B44" t="inlineStr">
+        <is>
+          <t>371</t>
+        </is>
+      </c>
+      <c r="C44" t="inlineStr">
+        <is>
+          <t>Российский государственный геологоразведочный университет имени Серго Орджоникидзе</t>
+        </is>
+      </c>
+    </row>
+    <row r="45">
+      <c r="A45" s="1" t="n">
+        <v>43</v>
+      </c>
+      <c r="B45" t="inlineStr">
+        <is>
+          <t>99</t>
+        </is>
+      </c>
+      <c r="C45" t="inlineStr">
+        <is>
+          <t>Институт физики Земли им. О.Ю. Шмидта РАН</t>
+        </is>
+      </c>
+    </row>
+    <row r="46">
+      <c r="A46" s="1" t="n">
+        <v>44</v>
+      </c>
+      <c r="B46" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> </t>
+        </is>
+      </c>
+      <c r="C46" t="inlineStr">
+        <is>
+          <t>18 Vinogradnaya Street, Alushta, 298517</t>
+        </is>
+      </c>
+    </row>
+    <row r="47">
+      <c r="A47" s="1" t="n">
+        <v>45</v>
+      </c>
+      <c r="B47" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> </t>
+        </is>
+      </c>
+      <c r="C47" t="inlineStr">
+        <is>
+          <t>Weatherford</t>
+        </is>
+      </c>
+    </row>
+    <row r="48">
+      <c r="A48" s="1" t="n">
+        <v>46</v>
+      </c>
+      <c r="B48" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> </t>
+        </is>
+      </c>
+      <c r="C48" t="inlineStr">
+        <is>
+          <t>Institute of Energy Strategy</t>
+        </is>
+      </c>
+    </row>
+    <row r="49">
+      <c r="A49" s="1" t="n">
+        <v>47</v>
+      </c>
+      <c r="B49" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> </t>
+        </is>
+      </c>
+      <c r="C49" t="inlineStr">
+        <is>
+          <t>ООО НТФ "Атомбиотех"</t>
+        </is>
+      </c>
+    </row>
+    <row r="50">
+      <c r="A50" s="1" t="n">
+        <v>48</v>
+      </c>
+      <c r="B50" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> </t>
+        </is>
+      </c>
+      <c r="C50" t="inlineStr">
+        <is>
+          <t>Oil and Gas Research Institute Russian Academy of Sciences (IPNG RAS)</t>
+        </is>
+      </c>
+    </row>
+    <row r="51">
+      <c r="A51" s="1" t="n">
+        <v>49</v>
+      </c>
+      <c r="B51" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> </t>
+        </is>
+      </c>
+      <c r="C51" t="inlineStr">
+        <is>
+          <t>IPNG RAN</t>
+        </is>
+      </c>
+    </row>
+    <row r="52">
+      <c r="A52" s="1" t="n">
+        <v>50</v>
+      </c>
+      <c r="B52" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> </t>
+        </is>
+      </c>
+      <c r="C52" t="inlineStr">
+        <is>
+          <t>Institute of Oil and Gas Problems of the Russian Academy of Sciences</t>
+        </is>
+      </c>
+    </row>
+    <row r="53">
+      <c r="A53" s="1" t="n">
+        <v>51</v>
+      </c>
+      <c r="B53" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> </t>
+        </is>
+      </c>
+      <c r="C53" t="inlineStr">
+        <is>
+          <t>АО "Томский научно-исследовательский и проектный институт нефти и газа" (АО "ТомскНИПИнефть")</t>
+        </is>
+      </c>
+    </row>
+    <row r="54">
+      <c r="A54" s="1" t="n">
+        <v>52</v>
+      </c>
+      <c r="B54" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> </t>
+        </is>
+      </c>
+      <c r="C54" t="inlineStr">
+        <is>
+          <t>Institute of Solid State Physics|Russian Academy of Sciences Academician</t>
+        </is>
+      </c>
+    </row>
+    <row r="55">
+      <c r="A55" s="1" t="n">
+        <v>53</v>
+      </c>
+      <c r="B55" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> </t>
+        </is>
+      </c>
+      <c r="C55" t="inlineStr">
+        <is>
+          <t>ООО «Тюменский институт нефти и газа»</t>
+        </is>
+      </c>
+    </row>
+    <row r="56">
+      <c r="A56" s="1" t="n">
+        <v>54</v>
+      </c>
+      <c r="B56" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> </t>
+        </is>
+      </c>
+      <c r="C56" t="inlineStr">
+        <is>
+          <t>Группа компаний ITPS</t>
+        </is>
+      </c>
+    </row>
+    <row r="57">
+      <c r="A57" s="1" t="n">
+        <v>55</v>
+      </c>
+      <c r="B57" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> </t>
+        </is>
+      </c>
+      <c r="C57" t="inlineStr">
+        <is>
+          <t>Wildcat Technologies LLC</t>
+        </is>
+      </c>
+    </row>
+    <row r="58">
+      <c r="A58" s="1" t="n">
+        <v>56</v>
+      </c>
+      <c r="B58" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> </t>
+        </is>
+      </c>
+      <c r="C58" t="inlineStr">
+        <is>
+          <t>Хромос Инжиниринг</t>
+        </is>
+      </c>
+    </row>
+    <row r="59">
+      <c r="A59" s="1" t="n">
+        <v>57</v>
+      </c>
+      <c r="B59" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> </t>
+        </is>
+      </c>
+      <c r="C59" t="inlineStr">
+        <is>
+          <t>Department of Biotechnology|I. M. Sechenov First Moscow State Medical University</t>
+        </is>
+      </c>
+    </row>
+    <row r="60">
+      <c r="A60" s="1" t="n">
+        <v>58</v>
+      </c>
+      <c r="B60" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> </t>
+        </is>
+      </c>
+      <c r="C60" t="inlineStr">
+        <is>
+          <t>Landau Institute for Theoretical Physics of the RAS</t>
+        </is>
+      </c>
+    </row>
+    <row r="61">
+      <c r="A61" s="1" t="n">
+        <v>59</v>
+      </c>
+      <c r="B61" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> </t>
+        </is>
+      </c>
+      <c r="C61" t="inlineStr">
+        <is>
+          <t>Institute of Solid State Physics of the RAS</t>
+        </is>
+      </c>
+    </row>
+    <row r="62">
+      <c r="A62" s="1" t="n">
+        <v>60</v>
+      </c>
+      <c r="B62" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> </t>
+        </is>
+      </c>
+      <c r="C62" t="inlineStr">
+        <is>
+          <t>ООО "Хромос Инжиниринг"</t>
+        </is>
+      </c>
+    </row>
+    <row r="63">
+      <c r="A63" s="1" t="n">
+        <v>61</v>
+      </c>
+      <c r="B63" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> </t>
+        </is>
+      </c>
+      <c r="C63" t="inlineStr">
+        <is>
+          <t>Gazprom Export</t>
+        </is>
+      </c>
+    </row>
+    <row r="64">
+      <c r="A64" s="1" t="n">
+        <v>62</v>
+      </c>
+      <c r="B64" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> </t>
+        </is>
+      </c>
+      <c r="C64" t="inlineStr">
+        <is>
+          <t>Scientific Council of RAS on System Research in Energy</t>
+        </is>
+      </c>
+    </row>
+    <row r="65">
+      <c r="A65" s="1" t="n">
+        <v>63</v>
+      </c>
+      <c r="B65" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> </t>
+        </is>
+      </c>
+      <c r="C65" t="inlineStr">
+        <is>
+          <t>Nansen Environmental and Remote Sensing Centre|Bjerknes Centre for Climate Research</t>
+        </is>
+      </c>
+    </row>
+    <row r="66">
+      <c r="A66" s="1" t="n">
+        <v>64</v>
+      </c>
+      <c r="B66" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> </t>
+        </is>
+      </c>
+      <c r="C66" t="inlineStr">
+        <is>
+          <t>Department of Geography|The George Washington University</t>
+        </is>
+      </c>
+    </row>
+    <row r="67">
+      <c r="A67" s="1" t="n">
+        <v>65</v>
+      </c>
+      <c r="B67" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> </t>
+        </is>
+      </c>
+      <c r="C67" t="inlineStr">
+        <is>
+          <t>Межотраслевой экспертно - аналитический центр Союза Нефтегазопромышленников России</t>
+        </is>
+      </c>
+    </row>
+    <row r="68">
+      <c r="A68" s="1" t="n">
+        <v>66</v>
+      </c>
+      <c r="B68" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> </t>
+        </is>
+      </c>
+      <c r="C68" t="inlineStr">
+        <is>
+          <t>ООО «Красноярскгазпром нефтегазпроект»</t>
+        </is>
+      </c>
+    </row>
+    <row r="69">
+      <c r="A69" s="1" t="n">
+        <v>67</v>
+      </c>
+      <c r="B69" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> </t>
+        </is>
+      </c>
+      <c r="C69" t="inlineStr">
+        <is>
+          <t>ООО «КБ Стрелка»</t>
+        </is>
+      </c>
+    </row>
+    <row r="70">
+      <c r="A70" s="1" t="n">
+        <v>68</v>
+      </c>
+      <c r="B70" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> </t>
+        </is>
+      </c>
+      <c r="C70" t="inlineStr">
         <is>
           <t>ООО Тимано-Печорский научно-исследовательский центр (ООО «ТПНИЦ»)</t>
         </is>

</xml_diff>

<commit_message>
added user template export to excel,added table for adding one row in DB,delete number of affilations from export, addded progressbar for import
</commit_message>
<xml_diff>
--- a/one_unique_organisations.xlsx
+++ b/one_unique_organisations.xlsx
@@ -451,7 +451,7 @@
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>11374</t>
+          <t>533</t>
         </is>
       </c>
       <c r="C2" t="inlineStr">
@@ -466,7 +466,7 @@
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>132</t>
+          <t>898</t>
         </is>
       </c>
       <c r="C3" t="inlineStr">
@@ -481,7 +481,7 @@
       </c>
       <c r="B4" t="inlineStr">
         <is>
-          <t>13814</t>
+          <t>870</t>
         </is>
       </c>
       <c r="C4" t="inlineStr">
@@ -496,7 +496,7 @@
       </c>
       <c r="B5" t="inlineStr">
         <is>
-          <t>14552</t>
+          <t>848</t>
         </is>
       </c>
       <c r="C5" t="inlineStr">
@@ -511,7 +511,7 @@
       </c>
       <c r="B6" t="inlineStr">
         <is>
-          <t>176</t>
+          <t>80</t>
         </is>
       </c>
       <c r="C6" t="inlineStr">
@@ -526,7 +526,7 @@
       </c>
       <c r="B7" t="inlineStr">
         <is>
-          <t>2268</t>
+          <t>7655</t>
         </is>
       </c>
       <c r="C7" t="inlineStr">
@@ -541,7 +541,7 @@
       </c>
       <c r="B8" t="inlineStr">
         <is>
-          <t>364</t>
+          <t>734</t>
         </is>
       </c>
       <c r="C8" t="inlineStr">
@@ -556,7 +556,7 @@
       </c>
       <c r="B9" t="inlineStr">
         <is>
-          <t>3966</t>
+          <t>7109</t>
         </is>
       </c>
       <c r="C9" t="inlineStr">
@@ -571,7 +571,7 @@
       </c>
       <c r="B10" t="inlineStr">
         <is>
-          <t>440</t>
+          <t>6939</t>
         </is>
       </c>
       <c r="C10" t="inlineStr">
@@ -586,12 +586,12 @@
       </c>
       <c r="B11" t="inlineStr">
         <is>
-          <t>4493</t>
+          <t>570</t>
         </is>
       </c>
       <c r="C11" t="inlineStr">
         <is>
-          <t>ООО «Тюменский нефтяной научный центр»</t>
+          <t>ИПНГ РАН</t>
         </is>
       </c>
     </row>
@@ -601,7 +601,7 @@
       </c>
       <c r="B12" t="inlineStr">
         <is>
-          <t>4750</t>
+          <t>549</t>
         </is>
       </c>
       <c r="C12" t="inlineStr">
@@ -631,7 +631,7 @@
       </c>
       <c r="B14" t="inlineStr">
         <is>
-          <t>533</t>
+          <t>11374</t>
         </is>
       </c>
       <c r="C14" t="inlineStr">
@@ -646,7 +646,7 @@
       </c>
       <c r="B15" t="inlineStr">
         <is>
-          <t>549</t>
+          <t>4750</t>
         </is>
       </c>
       <c r="C15" t="inlineStr">
@@ -661,12 +661,12 @@
       </c>
       <c r="B16" t="inlineStr">
         <is>
-          <t>570</t>
+          <t>4493</t>
         </is>
       </c>
       <c r="C16" t="inlineStr">
         <is>
-          <t>ИПНГ РАН</t>
+          <t>Oil and Gas Research Institute|Russian Academy of Sciences (OGRI RAS)</t>
         </is>
       </c>
     </row>
@@ -676,7 +676,7 @@
       </c>
       <c r="B17" t="inlineStr">
         <is>
-          <t>6939</t>
+          <t>440</t>
         </is>
       </c>
       <c r="C17" t="inlineStr">
@@ -691,7 +691,7 @@
       </c>
       <c r="B18" t="inlineStr">
         <is>
-          <t>7109</t>
+          <t>3966</t>
         </is>
       </c>
       <c r="C18" t="inlineStr">
@@ -706,7 +706,7 @@
       </c>
       <c r="B19" t="inlineStr">
         <is>
-          <t>734</t>
+          <t>364</t>
         </is>
       </c>
       <c r="C19" t="inlineStr">
@@ -721,7 +721,7 @@
       </c>
       <c r="B20" t="inlineStr">
         <is>
-          <t>7655</t>
+          <t>2268</t>
         </is>
       </c>
       <c r="C20" t="inlineStr">
@@ -736,7 +736,7 @@
       </c>
       <c r="B21" t="inlineStr">
         <is>
-          <t>80</t>
+          <t>176</t>
         </is>
       </c>
       <c r="C21" t="inlineStr">
@@ -751,7 +751,7 @@
       </c>
       <c r="B22" t="inlineStr">
         <is>
-          <t>848</t>
+          <t>14552</t>
         </is>
       </c>
       <c r="C22" t="inlineStr">
@@ -766,7 +766,7 @@
       </c>
       <c r="B23" t="inlineStr">
         <is>
-          <t>870</t>
+          <t>13814</t>
         </is>
       </c>
       <c r="C23" t="inlineStr">
@@ -781,7 +781,7 @@
       </c>
       <c r="B24" t="inlineStr">
         <is>
-          <t>898</t>
+          <t>132</t>
         </is>
       </c>
       <c r="C24" t="inlineStr">

</xml_diff>